<commit_message>
release 0.2.1 update test coverage badge update indevidual Assessment
</commit_message>
<xml_diff>
--- a/assessment/Team-3-Individual-Assessment.xlsx
+++ b/assessment/Team-3-Individual-Assessment.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reda/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reda/IdeaProjects/devops-project/assessment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5ECBF67A-1995-8245-AFBD-0DA38A187E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBC1BEA-0EB2-1744-A8CD-58B95285F448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45140" yWindow="5260" windowWidth="28040" windowHeight="17440" xr2:uid="{5B903C90-01EA-5C44-B7D7-CD7D5703BC82}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20520" xr2:uid="{5B903C90-01EA-5C44-B7D7-CD7D5703BC82}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -121,18 +121,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -472,7 +469,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -501,6 +498,9 @@
       <c r="B2">
         <v>16.6666667</v>
       </c>
+      <c r="C2">
+        <v>16.6666667</v>
+      </c>
       <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
@@ -512,15 +512,21 @@
       <c r="B3">
         <v>16.6666667</v>
       </c>
+      <c r="C3">
+        <v>16.6666667</v>
+      </c>
       <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>40799947</v>
       </c>
       <c r="B4">
+        <v>16.6666667</v>
+      </c>
+      <c r="C4">
         <v>16.6666667</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -534,6 +540,9 @@
       <c r="B5">
         <v>16.6666667</v>
       </c>
+      <c r="C5">
+        <v>16.6666667</v>
+      </c>
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
@@ -545,6 +554,9 @@
       <c r="B6">
         <v>16.6666667</v>
       </c>
+      <c r="C6">
+        <v>16.6666667</v>
+      </c>
       <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
@@ -556,6 +568,9 @@
       <c r="B7">
         <v>16.6666667</v>
       </c>
+      <c r="C7">
+        <v>16.6666667</v>
+      </c>
       <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
@@ -569,8 +584,8 @@
         <v>100</v>
       </c>
       <c r="C8">
-        <f>SUM(C2:C7)</f>
-        <v>0</v>
+        <f>ROUND(SUM(C2:C7),2)</f>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>